<commit_message>
updated scenarios with target trial approach
</commit_message>
<xml_diff>
--- a/data/scenarios.xlsx
+++ b/data/scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corinneriddell/Documents/repos/TWFE-simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BE902B-EAF0-C34C-AA10-5196811C2EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0827C056-C2D5-2D44-9B3C-8F0939EBD115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36200" yWindow="-6640" windowWidth="30240" windowHeight="18880" activeTab="10" xr2:uid="{3A84A3DE-CD8F-5C4B-BB69-5AB88BC02DD1}"/>
+    <workbookView xWindow="-36200" yWindow="500" windowWidth="30240" windowHeight="18880" activeTab="8" xr2:uid="{3A84A3DE-CD8F-5C4B-BB69-5AB88BC02DD1}"/>
   </bookViews>
   <sheets>
     <sheet name="scen1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="8">
   <si>
     <t>state</t>
   </si>
@@ -64,11 +62,20 @@
   <si>
     <t>time_first_treat</t>
   </si>
+  <si>
+    <t>time_as_date</t>
+  </si>
+  <si>
+    <t>time_first_trt_date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -129,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -138,6 +145,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3393,7 +3401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614FFDD6-16D5-BA47-8A1C-7C7CB4FDA225}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -7235,18 +7243,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F50E3BD-804D-9843-BE18-BD1661C90A82}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G2" sqref="G2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7265,8 +7276,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7285,8 +7302,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="8">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7305,8 +7325,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="8">
+        <v>42036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -7325,8 +7348,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="8">
+        <v>42064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -7345,8 +7371,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="8">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -7365,8 +7394,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -7385,8 +7417,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -7405,8 +7440,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="8">
+        <v>42186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -7425,8 +7463,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="8">
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -7445,8 +7486,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="8">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -7465,8 +7509,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="8">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -7486,8 +7533,14 @@
       <c r="F12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="8">
+        <v>42005</v>
+      </c>
+      <c r="H12" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -7507,8 +7560,14 @@
       <c r="F13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="8">
+        <v>42036</v>
+      </c>
+      <c r="H13" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -7528,8 +7587,14 @@
       <c r="F14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="8">
+        <v>42064</v>
+      </c>
+      <c r="H14" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -7549,8 +7614,14 @@
       <c r="F15">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="8">
+        <v>42095</v>
+      </c>
+      <c r="H15" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -7570,8 +7641,14 @@
       <c r="F16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="8">
+        <v>42125</v>
+      </c>
+      <c r="H16" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -7591,8 +7668,14 @@
       <c r="F17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="8">
+        <v>42156</v>
+      </c>
+      <c r="H17" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -7612,8 +7695,14 @@
       <c r="F18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="8">
+        <v>42186</v>
+      </c>
+      <c r="H18" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -7633,8 +7722,14 @@
       <c r="F19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="8">
+        <v>42217</v>
+      </c>
+      <c r="H19" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -7654,8 +7749,14 @@
       <c r="F20">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="8">
+        <v>42248</v>
+      </c>
+      <c r="H20" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -7675,8 +7776,14 @@
       <c r="F21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="8">
+        <v>42278</v>
+      </c>
+      <c r="H21" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -7696,8 +7803,14 @@
       <c r="F22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="8">
+        <v>42005</v>
+      </c>
+      <c r="H22" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -7717,8 +7830,14 @@
       <c r="F23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="8">
+        <v>42036</v>
+      </c>
+      <c r="H23" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -7738,8 +7857,14 @@
       <c r="F24">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="8">
+        <v>42064</v>
+      </c>
+      <c r="H24" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -7759,8 +7884,14 @@
       <c r="F25">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="8">
+        <v>42095</v>
+      </c>
+      <c r="H25" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -7780,8 +7911,14 @@
       <c r="F26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="8">
+        <v>42125</v>
+      </c>
+      <c r="H26" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -7801,8 +7938,14 @@
       <c r="F27">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="8">
+        <v>42156</v>
+      </c>
+      <c r="H27" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -7822,8 +7965,14 @@
       <c r="F28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="8">
+        <v>42186</v>
+      </c>
+      <c r="H28" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -7843,8 +7992,14 @@
       <c r="F29">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="8">
+        <v>42217</v>
+      </c>
+      <c r="H29" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -7864,8 +8019,14 @@
       <c r="F30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="8">
+        <v>42248</v>
+      </c>
+      <c r="H30" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -7885,8 +8046,14 @@
       <c r="F31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="8">
+        <v>42278</v>
+      </c>
+      <c r="H31" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -7906,8 +8073,14 @@
       <c r="F32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="8">
+        <v>42005</v>
+      </c>
+      <c r="H32" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -7927,8 +8100,14 @@
       <c r="F33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="8">
+        <v>42036</v>
+      </c>
+      <c r="H33" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -7948,8 +8127,14 @@
       <c r="F34">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="8">
+        <v>42064</v>
+      </c>
+      <c r="H34" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -7969,8 +8154,14 @@
       <c r="F35">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="8">
+        <v>42095</v>
+      </c>
+      <c r="H35" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -7990,8 +8181,14 @@
       <c r="F36">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="8">
+        <v>42125</v>
+      </c>
+      <c r="H36" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -8011,8 +8208,14 @@
       <c r="F37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="8">
+        <v>42156</v>
+      </c>
+      <c r="H37" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -8032,8 +8235,14 @@
       <c r="F38">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" s="8">
+        <v>42186</v>
+      </c>
+      <c r="H38" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -8053,8 +8262,14 @@
       <c r="F39">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" s="8">
+        <v>42217</v>
+      </c>
+      <c r="H39" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -8074,8 +8289,14 @@
       <c r="F40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="8">
+        <v>42248</v>
+      </c>
+      <c r="H40" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -8094,6 +8315,12 @@
       </c>
       <c r="F41">
         <v>6</v>
+      </c>
+      <c r="G41" s="8">
+        <v>42278</v>
+      </c>
+      <c r="H41" s="8">
+        <v>42156</v>
       </c>
     </row>
   </sheetData>
@@ -8103,19 +8330,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F2608B-013F-F240-B42A-42C2F56EDC88}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8134,8 +8363,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8154,8 +8389,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="8">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8174,8 +8412,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="8">
+        <v>42036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -8194,8 +8435,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="8">
+        <v>42064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -8214,8 +8458,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="8">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -8234,8 +8481,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -8254,8 +8504,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -8274,8 +8527,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="8">
+        <v>42186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -8294,8 +8550,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="8">
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -8314,8 +8573,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="8">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -8334,8 +8596,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="8">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -8354,8 +8619,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="8">
+        <v>42309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -8374,8 +8642,11 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -8394,8 +8665,11 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="8">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -8414,8 +8688,11 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="8">
+        <v>42401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -8434,8 +8711,11 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="8">
+        <v>42430</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -8454,8 +8734,11 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="8">
+        <v>42461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -8474,8 +8757,11 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="8">
+        <v>42491</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -8494,8 +8780,11 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="8">
+        <v>42522</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -8514,8 +8803,11 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="8">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -8534,8 +8826,11 @@
       <c r="F21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="8">
+        <v>42583</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -8555,8 +8850,11 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="8">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -8576,8 +8874,11 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="8">
+        <v>42036</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -8597,8 +8898,11 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="8">
+        <v>42064</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -8618,8 +8922,11 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="8">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -8639,8 +8946,11 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -8660,8 +8970,11 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -8681,8 +8994,11 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="8">
+        <v>42186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -8702,8 +9018,11 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="8">
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -8723,8 +9042,11 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="8">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -8744,8 +9066,11 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="8">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -8765,8 +9090,11 @@
       <c r="F32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="8">
+        <v>42309</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -8786,8 +9114,11 @@
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2</v>
       </c>
@@ -8807,8 +9138,11 @@
       <c r="F34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="8">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -8828,8 +9162,11 @@
       <c r="F35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="8">
+        <v>42401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
@@ -8849,8 +9186,11 @@
       <c r="F36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="8">
+        <v>42430</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2</v>
       </c>
@@ -8870,8 +9210,11 @@
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="8">
+        <v>42461</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2</v>
       </c>
@@ -8891,8 +9234,11 @@
       <c r="F38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" s="8">
+        <v>42491</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
@@ -8912,8 +9258,11 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" s="8">
+        <v>42522</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -8933,8 +9282,11 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="8">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
@@ -8954,8 +9306,11 @@
       <c r="F41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" s="8">
+        <v>42583</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -8975,8 +9330,14 @@
       <c r="F42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" s="8">
+        <v>42005</v>
+      </c>
+      <c r="H42" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -8996,8 +9357,14 @@
       <c r="F43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" s="8">
+        <v>42036</v>
+      </c>
+      <c r="H43" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
@@ -9017,8 +9384,14 @@
       <c r="F44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" s="8">
+        <v>42064</v>
+      </c>
+      <c r="H44" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -9038,8 +9411,14 @@
       <c r="F45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" s="8">
+        <v>42095</v>
+      </c>
+      <c r="H45" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -9059,8 +9438,14 @@
       <c r="F46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" s="8">
+        <v>42125</v>
+      </c>
+      <c r="H46" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
@@ -9080,8 +9465,14 @@
       <c r="F47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" s="8">
+        <v>42156</v>
+      </c>
+      <c r="H47" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3</v>
       </c>
@@ -9101,8 +9492,14 @@
       <c r="F48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="8">
+        <v>42186</v>
+      </c>
+      <c r="H48" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -9122,8 +9519,14 @@
       <c r="F49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="8">
+        <v>42217</v>
+      </c>
+      <c r="H49" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -9143,8 +9546,14 @@
       <c r="F50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" s="8">
+        <v>42248</v>
+      </c>
+      <c r="H50" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -9164,8 +9573,14 @@
       <c r="F51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" s="8">
+        <v>42278</v>
+      </c>
+      <c r="H51" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -9185,8 +9600,14 @@
       <c r="F52">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" s="8">
+        <v>42309</v>
+      </c>
+      <c r="H52" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -9206,8 +9627,14 @@
       <c r="F53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" s="8">
+        <v>42339</v>
+      </c>
+      <c r="H53" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
@@ -9227,8 +9654,14 @@
       <c r="F54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" s="8">
+        <v>42370</v>
+      </c>
+      <c r="H54" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3</v>
       </c>
@@ -9248,8 +9681,14 @@
       <c r="F55">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" s="8">
+        <v>42401</v>
+      </c>
+      <c r="H55" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
@@ -9269,8 +9708,14 @@
       <c r="F56">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" s="8">
+        <v>42430</v>
+      </c>
+      <c r="H56" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3</v>
       </c>
@@ -9290,8 +9735,14 @@
       <c r="F57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" s="8">
+        <v>42461</v>
+      </c>
+      <c r="H57" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>3</v>
       </c>
@@ -9311,8 +9762,14 @@
       <c r="F58">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" s="8">
+        <v>42491</v>
+      </c>
+      <c r="H58" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>3</v>
       </c>
@@ -9332,8 +9789,14 @@
       <c r="F59">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" s="8">
+        <v>42522</v>
+      </c>
+      <c r="H59" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>3</v>
       </c>
@@ -9353,8 +9816,14 @@
       <c r="F60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" s="8">
+        <v>42552</v>
+      </c>
+      <c r="H60" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>3</v>
       </c>
@@ -9374,8 +9843,14 @@
       <c r="F61">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" s="8">
+        <v>42583</v>
+      </c>
+      <c r="H61" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>4</v>
       </c>
@@ -9395,8 +9870,14 @@
       <c r="F62">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62" s="8">
+        <v>42005</v>
+      </c>
+      <c r="H62" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>4</v>
       </c>
@@ -9416,8 +9897,14 @@
       <c r="F63">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" s="8">
+        <v>42036</v>
+      </c>
+      <c r="H63" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>4</v>
       </c>
@@ -9437,8 +9924,14 @@
       <c r="F64">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64" s="8">
+        <v>42064</v>
+      </c>
+      <c r="H64" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>4</v>
       </c>
@@ -9458,8 +9951,14 @@
       <c r="F65">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65" s="8">
+        <v>42095</v>
+      </c>
+      <c r="H65" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>4</v>
       </c>
@@ -9479,8 +9978,14 @@
       <c r="F66">
         <v>12</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" s="8">
+        <v>42125</v>
+      </c>
+      <c r="H66" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>4</v>
       </c>
@@ -9500,8 +10005,14 @@
       <c r="F67">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" s="8">
+        <v>42156</v>
+      </c>
+      <c r="H67" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>4</v>
       </c>
@@ -9521,8 +10032,14 @@
       <c r="F68">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68" s="8">
+        <v>42186</v>
+      </c>
+      <c r="H68" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>4</v>
       </c>
@@ -9542,8 +10059,14 @@
       <c r="F69">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69" s="8">
+        <v>42217</v>
+      </c>
+      <c r="H69" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>4</v>
       </c>
@@ -9563,8 +10086,14 @@
       <c r="F70">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70" s="8">
+        <v>42248</v>
+      </c>
+      <c r="H70" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>4</v>
       </c>
@@ -9584,8 +10113,14 @@
       <c r="F71">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71" s="8">
+        <v>42278</v>
+      </c>
+      <c r="H71" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>4</v>
       </c>
@@ -9605,8 +10140,14 @@
       <c r="F72">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72" s="8">
+        <v>42309</v>
+      </c>
+      <c r="H72" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>4</v>
       </c>
@@ -9626,8 +10167,14 @@
       <c r="F73">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73" s="8">
+        <v>42339</v>
+      </c>
+      <c r="H73" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>4</v>
       </c>
@@ -9647,8 +10194,14 @@
       <c r="F74">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74" s="8">
+        <v>42370</v>
+      </c>
+      <c r="H74" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>4</v>
       </c>
@@ -9668,8 +10221,14 @@
       <c r="F75">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75" s="8">
+        <v>42401</v>
+      </c>
+      <c r="H75" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>4</v>
       </c>
@@ -9689,8 +10248,14 @@
       <c r="F76">
         <v>12</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76" s="8">
+        <v>42430</v>
+      </c>
+      <c r="H76" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>4</v>
       </c>
@@ -9710,8 +10275,14 @@
       <c r="F77">
         <v>12</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77" s="8">
+        <v>42461</v>
+      </c>
+      <c r="H77" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>4</v>
       </c>
@@ -9731,8 +10302,14 @@
       <c r="F78">
         <v>12</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78" s="8">
+        <v>42491</v>
+      </c>
+      <c r="H78" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>4</v>
       </c>
@@ -9752,8 +10329,14 @@
       <c r="F79">
         <v>12</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79" s="8">
+        <v>42522</v>
+      </c>
+      <c r="H79" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>4</v>
       </c>
@@ -9773,8 +10356,14 @@
       <c r="F80">
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" s="8">
+        <v>42552</v>
+      </c>
+      <c r="H80" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>4</v>
       </c>
@@ -9793,6 +10382,12 @@
       </c>
       <c r="F81">
         <v>12</v>
+      </c>
+      <c r="G81" s="8">
+        <v>42583</v>
+      </c>
+      <c r="H81" s="8">
+        <v>42339</v>
       </c>
     </row>
   </sheetData>
@@ -9804,17 +10399,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3433CF-54DF-E64E-AB09-C6F8EBF063B6}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I82" sqref="I82:I83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9833,8 +10430,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9853,8 +10456,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="8">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -9873,8 +10479,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="8">
+        <v>42036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -9893,8 +10502,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="8">
+        <v>42064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -9913,8 +10525,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="8">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -9933,8 +10548,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -9953,8 +10571,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -9973,8 +10594,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="8">
+        <v>42186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -9993,8 +10617,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="8">
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -10013,8 +10640,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="8">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -10033,8 +10663,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="8">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -10053,8 +10686,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="8">
+        <v>42309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -10073,8 +10709,11 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -10093,8 +10732,11 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="8">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -10113,8 +10755,11 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="8">
+        <v>42401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -10133,8 +10778,11 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="8">
+        <v>42430</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -10153,8 +10801,11 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="8">
+        <v>42461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -10173,8 +10824,11 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="8">
+        <v>42491</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -10193,8 +10847,11 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="8">
+        <v>42522</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -10213,8 +10870,11 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="8">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -10233,8 +10893,11 @@
       <c r="F21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="8">
+        <v>42583</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -10254,8 +10917,11 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="8">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -10275,8 +10941,11 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="8">
+        <v>42036</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -10296,8 +10965,11 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="8">
+        <v>42064</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -10317,8 +10989,11 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="8">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -10338,8 +11013,11 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -10359,8 +11037,11 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -10380,8 +11061,11 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="8">
+        <v>42186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -10401,8 +11085,11 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="8">
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -10422,8 +11109,11 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="8">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -10443,8 +11133,11 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="8">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -10464,6 +11157,9 @@
       <c r="F32">
         <v>0</v>
       </c>
+      <c r="G32" s="8">
+        <v>42309</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -10485,6 +11181,9 @@
       <c r="F33">
         <v>0</v>
       </c>
+      <c r="G33" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -10506,6 +11205,9 @@
       <c r="F34">
         <v>0</v>
       </c>
+      <c r="G34" s="8">
+        <v>42370</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
@@ -10527,6 +11229,9 @@
       <c r="F35">
         <v>0</v>
       </c>
+      <c r="G35" s="8">
+        <v>42401</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
@@ -10548,6 +11253,9 @@
       <c r="F36">
         <v>0</v>
       </c>
+      <c r="G36" s="8">
+        <v>42430</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -10569,6 +11277,9 @@
       <c r="F37">
         <v>0</v>
       </c>
+      <c r="G37" s="8">
+        <v>42461</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
@@ -10590,6 +11301,9 @@
       <c r="F38">
         <v>0</v>
       </c>
+      <c r="G38" s="8">
+        <v>42491</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -10611,6 +11325,9 @@
       <c r="F39">
         <v>0</v>
       </c>
+      <c r="G39" s="8">
+        <v>42522</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
@@ -10632,8 +11349,9 @@
       <c r="F40">
         <v>0</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="G40" s="8">
+        <v>42552</v>
+      </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
@@ -10657,8 +11375,9 @@
       <c r="F41">
         <v>0</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="G41" s="8">
+        <v>42583</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
@@ -10682,8 +11401,12 @@
       <c r="F42">
         <v>5</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="G42" s="8">
+        <v>42005</v>
+      </c>
+      <c r="H42" s="8">
+        <v>42125</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
@@ -10707,8 +11430,12 @@
       <c r="F43">
         <v>5</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="G43" s="8">
+        <v>42036</v>
+      </c>
+      <c r="H43" s="8">
+        <v>42125</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
@@ -10732,8 +11459,12 @@
       <c r="F44">
         <v>5</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="G44" s="8">
+        <v>42064</v>
+      </c>
+      <c r="H44" s="8">
+        <v>42125</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
@@ -10757,8 +11488,12 @@
       <c r="F45">
         <v>5</v>
       </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
+      <c r="G45" s="8">
+        <v>42095</v>
+      </c>
+      <c r="H45" s="8">
+        <v>42125</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
@@ -10782,8 +11517,12 @@
       <c r="F46">
         <v>5</v>
       </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+      <c r="G46" s="8">
+        <v>42125</v>
+      </c>
+      <c r="H46" s="8">
+        <v>42125</v>
+      </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
@@ -10807,8 +11546,12 @@
       <c r="F47">
         <v>5</v>
       </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+      <c r="G47" s="8">
+        <v>42156</v>
+      </c>
+      <c r="H47" s="8">
+        <v>42125</v>
+      </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
@@ -10832,8 +11575,12 @@
       <c r="F48">
         <v>5</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
+      <c r="G48" s="8">
+        <v>42186</v>
+      </c>
+      <c r="H48" s="8">
+        <v>42125</v>
+      </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
@@ -10857,8 +11604,12 @@
       <c r="F49">
         <v>5</v>
       </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="G49" s="8">
+        <v>42217</v>
+      </c>
+      <c r="H49" s="8">
+        <v>42125</v>
+      </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
@@ -10882,8 +11633,12 @@
       <c r="F50">
         <v>5</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+      <c r="G50" s="8">
+        <v>42248</v>
+      </c>
+      <c r="H50" s="8">
+        <v>42125</v>
+      </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
@@ -10907,8 +11662,12 @@
       <c r="F51">
         <v>5</v>
       </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="G51" s="8">
+        <v>42278</v>
+      </c>
+      <c r="H51" s="8">
+        <v>42125</v>
+      </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
@@ -10932,8 +11691,12 @@
       <c r="F52">
         <v>5</v>
       </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+      <c r="G52" s="8">
+        <v>42309</v>
+      </c>
+      <c r="H52" s="8">
+        <v>42125</v>
+      </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
@@ -10957,8 +11720,12 @@
       <c r="F53">
         <v>5</v>
       </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="G53" s="8">
+        <v>42339</v>
+      </c>
+      <c r="H53" s="8">
+        <v>42125</v>
+      </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
@@ -10982,8 +11749,12 @@
       <c r="F54">
         <v>5</v>
       </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="G54" s="8">
+        <v>42370</v>
+      </c>
+      <c r="H54" s="8">
+        <v>42125</v>
+      </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
@@ -11007,8 +11778,12 @@
       <c r="F55">
         <v>5</v>
       </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+      <c r="G55" s="8">
+        <v>42401</v>
+      </c>
+      <c r="H55" s="8">
+        <v>42125</v>
+      </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
@@ -11032,8 +11807,12 @@
       <c r="F56">
         <v>5</v>
       </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
+      <c r="G56" s="8">
+        <v>42430</v>
+      </c>
+      <c r="H56" s="8">
+        <v>42125</v>
+      </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
@@ -11057,8 +11836,12 @@
       <c r="F57">
         <v>5</v>
       </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
+      <c r="G57" s="8">
+        <v>42461</v>
+      </c>
+      <c r="H57" s="8">
+        <v>42125</v>
+      </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
@@ -11082,8 +11865,12 @@
       <c r="F58">
         <v>5</v>
       </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
+      <c r="G58" s="8">
+        <v>42491</v>
+      </c>
+      <c r="H58" s="8">
+        <v>42125</v>
+      </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
@@ -11107,8 +11894,12 @@
       <c r="F59">
         <v>5</v>
       </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
+      <c r="G59" s="8">
+        <v>42522</v>
+      </c>
+      <c r="H59" s="8">
+        <v>42125</v>
+      </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
@@ -11132,8 +11923,12 @@
       <c r="F60">
         <v>5</v>
       </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
+      <c r="G60" s="8">
+        <v>42552</v>
+      </c>
+      <c r="H60" s="8">
+        <v>42125</v>
+      </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
@@ -11157,8 +11952,12 @@
       <c r="F61">
         <v>5</v>
       </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
+      <c r="G61" s="8">
+        <v>42583</v>
+      </c>
+      <c r="H61" s="8">
+        <v>42125</v>
+      </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
@@ -11182,8 +11981,12 @@
       <c r="F62">
         <v>12</v>
       </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
+      <c r="G62" s="8">
+        <v>42005</v>
+      </c>
+      <c r="H62" s="8">
+        <v>42339</v>
+      </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
@@ -11207,8 +12010,12 @@
       <c r="F63">
         <v>12</v>
       </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
+      <c r="G63" s="8">
+        <v>42036</v>
+      </c>
+      <c r="H63" s="8">
+        <v>42339</v>
+      </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
@@ -11232,8 +12039,12 @@
       <c r="F64">
         <v>12</v>
       </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
+      <c r="G64" s="8">
+        <v>42064</v>
+      </c>
+      <c r="H64" s="8">
+        <v>42339</v>
+      </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
@@ -11257,8 +12068,12 @@
       <c r="F65">
         <v>12</v>
       </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
+      <c r="G65" s="8">
+        <v>42095</v>
+      </c>
+      <c r="H65" s="8">
+        <v>42339</v>
+      </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
@@ -11282,8 +12097,12 @@
       <c r="F66">
         <v>12</v>
       </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
+      <c r="G66" s="8">
+        <v>42125</v>
+      </c>
+      <c r="H66" s="8">
+        <v>42339</v>
+      </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
@@ -11307,8 +12126,12 @@
       <c r="F67">
         <v>12</v>
       </c>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
+      <c r="G67" s="8">
+        <v>42156</v>
+      </c>
+      <c r="H67" s="8">
+        <v>42339</v>
+      </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
@@ -11332,8 +12155,12 @@
       <c r="F68">
         <v>12</v>
       </c>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
+      <c r="G68" s="8">
+        <v>42186</v>
+      </c>
+      <c r="H68" s="8">
+        <v>42339</v>
+      </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
@@ -11357,8 +12184,12 @@
       <c r="F69">
         <v>12</v>
       </c>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
+      <c r="G69" s="8">
+        <v>42217</v>
+      </c>
+      <c r="H69" s="8">
+        <v>42339</v>
+      </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
@@ -11382,8 +12213,12 @@
       <c r="F70">
         <v>12</v>
       </c>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
+      <c r="G70" s="8">
+        <v>42248</v>
+      </c>
+      <c r="H70" s="8">
+        <v>42339</v>
+      </c>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
@@ -11407,8 +12242,12 @@
       <c r="F71">
         <v>12</v>
       </c>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
+      <c r="G71" s="8">
+        <v>42278</v>
+      </c>
+      <c r="H71" s="8">
+        <v>42339</v>
+      </c>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
@@ -11432,8 +12271,12 @@
       <c r="F72">
         <v>12</v>
       </c>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
+      <c r="G72" s="8">
+        <v>42309</v>
+      </c>
+      <c r="H72" s="8">
+        <v>42339</v>
+      </c>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
@@ -11457,8 +12300,12 @@
       <c r="F73">
         <v>12</v>
       </c>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
+      <c r="G73" s="8">
+        <v>42339</v>
+      </c>
+      <c r="H73" s="8">
+        <v>42339</v>
+      </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
@@ -11482,8 +12329,12 @@
       <c r="F74">
         <v>12</v>
       </c>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
+      <c r="G74" s="8">
+        <v>42370</v>
+      </c>
+      <c r="H74" s="8">
+        <v>42339</v>
+      </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
@@ -11507,8 +12358,12 @@
       <c r="F75">
         <v>12</v>
       </c>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
+      <c r="G75" s="8">
+        <v>42401</v>
+      </c>
+      <c r="H75" s="8">
+        <v>42339</v>
+      </c>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
@@ -11532,6 +12387,12 @@
       <c r="F76">
         <v>12</v>
       </c>
+      <c r="G76" s="8">
+        <v>42430</v>
+      </c>
+      <c r="H76" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
@@ -11553,6 +12414,12 @@
       <c r="F77">
         <v>12</v>
       </c>
+      <c r="G77" s="8">
+        <v>42461</v>
+      </c>
+      <c r="H77" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
@@ -11574,6 +12441,12 @@
       <c r="F78">
         <v>12</v>
       </c>
+      <c r="G78" s="8">
+        <v>42491</v>
+      </c>
+      <c r="H78" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
@@ -11595,6 +12468,12 @@
       <c r="F79">
         <v>12</v>
       </c>
+      <c r="G79" s="8">
+        <v>42522</v>
+      </c>
+      <c r="H79" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -11616,8 +12495,14 @@
       <c r="F80">
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" s="8">
+        <v>42552</v>
+      </c>
+      <c r="H80" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>4</v>
       </c>
@@ -11636,6 +12521,12 @@
       </c>
       <c r="F81">
         <v>12</v>
+      </c>
+      <c r="G81" s="8">
+        <v>42583</v>
+      </c>
+      <c r="H81" s="8">
+        <v>42339</v>
       </c>
     </row>
   </sheetData>
@@ -11647,17 +12538,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32EF42-1665-1742-8ED8-18BCC709F02B}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11676,8 +12569,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11696,8 +12595,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="8">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11716,8 +12618,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="8">
+        <v>42036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -11736,8 +12641,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="8">
+        <v>42064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -11756,8 +12664,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="8">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -11776,8 +12687,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -11796,8 +12710,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -11816,8 +12733,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="8">
+        <v>42186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -11836,8 +12756,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="8">
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -11856,8 +12779,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="8">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -11876,8 +12802,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="8">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -11896,8 +12825,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="8">
+        <v>42309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -11916,8 +12848,11 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -11936,8 +12871,11 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="8">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -11956,8 +12894,11 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="8">
+        <v>42401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -11976,8 +12917,11 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="8">
+        <v>42430</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -11996,8 +12940,11 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="8">
+        <v>42461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -12016,8 +12963,11 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="8">
+        <v>42491</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -12036,8 +12986,11 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="8">
+        <v>42522</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -12056,8 +13009,11 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="8">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -12076,8 +13032,11 @@
       <c r="F21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="8">
+        <v>42583</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -12097,8 +13056,11 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="8">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -12118,8 +13080,11 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="8">
+        <v>42036</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -12139,8 +13104,11 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="8">
+        <v>42064</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -12160,8 +13128,11 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="8">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -12181,8 +13152,11 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="8">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -12202,8 +13176,11 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="8">
+        <v>42156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -12223,8 +13200,11 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="8">
+        <v>42186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -12244,8 +13224,11 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="8">
+        <v>42217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -12265,8 +13248,11 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="8">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -12286,8 +13272,11 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="8">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -12307,6 +13296,9 @@
       <c r="F32">
         <v>0</v>
       </c>
+      <c r="G32" s="8">
+        <v>42309</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -12328,6 +13320,9 @@
       <c r="F33">
         <v>0</v>
       </c>
+      <c r="G33" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -12349,6 +13344,9 @@
       <c r="F34">
         <v>0</v>
       </c>
+      <c r="G34" s="8">
+        <v>42370</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
@@ -12370,6 +13368,9 @@
       <c r="F35">
         <v>0</v>
       </c>
+      <c r="G35" s="8">
+        <v>42401</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
@@ -12391,6 +13392,9 @@
       <c r="F36">
         <v>0</v>
       </c>
+      <c r="G36" s="8">
+        <v>42430</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -12412,6 +13416,9 @@
       <c r="F37">
         <v>0</v>
       </c>
+      <c r="G37" s="8">
+        <v>42461</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
@@ -12433,6 +13440,9 @@
       <c r="F38">
         <v>0</v>
       </c>
+      <c r="G38" s="8">
+        <v>42491</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -12454,6 +13464,9 @@
       <c r="F39">
         <v>0</v>
       </c>
+      <c r="G39" s="8">
+        <v>42522</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
@@ -12475,8 +13488,9 @@
       <c r="F40">
         <v>0</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="G40" s="8">
+        <v>42552</v>
+      </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
@@ -12500,8 +13514,9 @@
       <c r="F41">
         <v>0</v>
       </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="G41" s="8">
+        <v>42583</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
@@ -12525,8 +13540,12 @@
       <c r="F42">
         <v>5</v>
       </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="G42" s="8">
+        <v>42005</v>
+      </c>
+      <c r="H42" s="8">
+        <v>42125</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
@@ -12550,8 +13569,12 @@
       <c r="F43">
         <v>5</v>
       </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="G43" s="8">
+        <v>42036</v>
+      </c>
+      <c r="H43" s="8">
+        <v>42125</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
@@ -12575,8 +13598,12 @@
       <c r="F44">
         <v>5</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="G44" s="8">
+        <v>42064</v>
+      </c>
+      <c r="H44" s="8">
+        <v>42125</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
@@ -12600,8 +13627,12 @@
       <c r="F45">
         <v>5</v>
       </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
+      <c r="G45" s="8">
+        <v>42095</v>
+      </c>
+      <c r="H45" s="8">
+        <v>42125</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
@@ -12625,8 +13656,12 @@
       <c r="F46">
         <v>5</v>
       </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+      <c r="G46" s="8">
+        <v>42125</v>
+      </c>
+      <c r="H46" s="8">
+        <v>42125</v>
+      </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
@@ -12650,8 +13685,12 @@
       <c r="F47">
         <v>5</v>
       </c>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+      <c r="G47" s="8">
+        <v>42156</v>
+      </c>
+      <c r="H47" s="8">
+        <v>42125</v>
+      </c>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
@@ -12675,8 +13714,12 @@
       <c r="F48">
         <v>5</v>
       </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
+      <c r="G48" s="8">
+        <v>42186</v>
+      </c>
+      <c r="H48" s="8">
+        <v>42125</v>
+      </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
@@ -12700,8 +13743,12 @@
       <c r="F49">
         <v>5</v>
       </c>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="G49" s="8">
+        <v>42217</v>
+      </c>
+      <c r="H49" s="8">
+        <v>42125</v>
+      </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
@@ -12725,8 +13772,12 @@
       <c r="F50">
         <v>5</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+      <c r="G50" s="8">
+        <v>42248</v>
+      </c>
+      <c r="H50" s="8">
+        <v>42125</v>
+      </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
@@ -12750,8 +13801,12 @@
       <c r="F51">
         <v>5</v>
       </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="G51" s="8">
+        <v>42278</v>
+      </c>
+      <c r="H51" s="8">
+        <v>42125</v>
+      </c>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
@@ -12775,8 +13830,12 @@
       <c r="F52">
         <v>5</v>
       </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+      <c r="G52" s="8">
+        <v>42309</v>
+      </c>
+      <c r="H52" s="8">
+        <v>42125</v>
+      </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
@@ -12800,8 +13859,12 @@
       <c r="F53">
         <v>5</v>
       </c>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="G53" s="8">
+        <v>42339</v>
+      </c>
+      <c r="H53" s="8">
+        <v>42125</v>
+      </c>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
@@ -12825,8 +13888,12 @@
       <c r="F54">
         <v>5</v>
       </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="G54" s="8">
+        <v>42370</v>
+      </c>
+      <c r="H54" s="8">
+        <v>42125</v>
+      </c>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
@@ -12850,8 +13917,12 @@
       <c r="F55">
         <v>5</v>
       </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+      <c r="G55" s="8">
+        <v>42401</v>
+      </c>
+      <c r="H55" s="8">
+        <v>42125</v>
+      </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
@@ -12875,8 +13946,12 @@
       <c r="F56">
         <v>5</v>
       </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
+      <c r="G56" s="8">
+        <v>42430</v>
+      </c>
+      <c r="H56" s="8">
+        <v>42125</v>
+      </c>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
@@ -12900,8 +13975,12 @@
       <c r="F57">
         <v>5</v>
       </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
+      <c r="G57" s="8">
+        <v>42461</v>
+      </c>
+      <c r="H57" s="8">
+        <v>42125</v>
+      </c>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
@@ -12925,8 +14004,12 @@
       <c r="F58">
         <v>5</v>
       </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
+      <c r="G58" s="8">
+        <v>42491</v>
+      </c>
+      <c r="H58" s="8">
+        <v>42125</v>
+      </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
@@ -12950,8 +14033,12 @@
       <c r="F59">
         <v>5</v>
       </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
+      <c r="G59" s="8">
+        <v>42522</v>
+      </c>
+      <c r="H59" s="8">
+        <v>42125</v>
+      </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
@@ -12975,8 +14062,12 @@
       <c r="F60">
         <v>5</v>
       </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
+      <c r="G60" s="8">
+        <v>42552</v>
+      </c>
+      <c r="H60" s="8">
+        <v>42125</v>
+      </c>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
@@ -13000,8 +14091,12 @@
       <c r="F61">
         <v>5</v>
       </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
+      <c r="G61" s="8">
+        <v>42583</v>
+      </c>
+      <c r="H61" s="8">
+        <v>42125</v>
+      </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
@@ -13025,8 +14120,12 @@
       <c r="F62">
         <v>12</v>
       </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
+      <c r="G62" s="8">
+        <v>42005</v>
+      </c>
+      <c r="H62" s="8">
+        <v>42339</v>
+      </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
@@ -13050,8 +14149,12 @@
       <c r="F63">
         <v>12</v>
       </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
+      <c r="G63" s="8">
+        <v>42036</v>
+      </c>
+      <c r="H63" s="8">
+        <v>42339</v>
+      </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
@@ -13075,8 +14178,12 @@
       <c r="F64">
         <v>12</v>
       </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
+      <c r="G64" s="8">
+        <v>42064</v>
+      </c>
+      <c r="H64" s="8">
+        <v>42339</v>
+      </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
@@ -13100,8 +14207,12 @@
       <c r="F65">
         <v>12</v>
       </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
+      <c r="G65" s="8">
+        <v>42095</v>
+      </c>
+      <c r="H65" s="8">
+        <v>42339</v>
+      </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
@@ -13125,8 +14236,12 @@
       <c r="F66">
         <v>12</v>
       </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
+      <c r="G66" s="8">
+        <v>42125</v>
+      </c>
+      <c r="H66" s="8">
+        <v>42339</v>
+      </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
@@ -13150,8 +14265,12 @@
       <c r="F67">
         <v>12</v>
       </c>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
+      <c r="G67" s="8">
+        <v>42156</v>
+      </c>
+      <c r="H67" s="8">
+        <v>42339</v>
+      </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
@@ -13175,8 +14294,12 @@
       <c r="F68">
         <v>12</v>
       </c>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
+      <c r="G68" s="8">
+        <v>42186</v>
+      </c>
+      <c r="H68" s="8">
+        <v>42339</v>
+      </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
@@ -13200,8 +14323,12 @@
       <c r="F69">
         <v>12</v>
       </c>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
+      <c r="G69" s="8">
+        <v>42217</v>
+      </c>
+      <c r="H69" s="8">
+        <v>42339</v>
+      </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
@@ -13225,8 +14352,12 @@
       <c r="F70">
         <v>12</v>
       </c>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
+      <c r="G70" s="8">
+        <v>42248</v>
+      </c>
+      <c r="H70" s="8">
+        <v>42339</v>
+      </c>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
@@ -13250,8 +14381,12 @@
       <c r="F71">
         <v>12</v>
       </c>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
+      <c r="G71" s="8">
+        <v>42278</v>
+      </c>
+      <c r="H71" s="8">
+        <v>42339</v>
+      </c>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
@@ -13275,8 +14410,12 @@
       <c r="F72">
         <v>12</v>
       </c>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
+      <c r="G72" s="8">
+        <v>42309</v>
+      </c>
+      <c r="H72" s="8">
+        <v>42339</v>
+      </c>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
@@ -13300,8 +14439,12 @@
       <c r="F73">
         <v>12</v>
       </c>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
+      <c r="G73" s="8">
+        <v>42339</v>
+      </c>
+      <c r="H73" s="8">
+        <v>42339</v>
+      </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
@@ -13325,8 +14468,12 @@
       <c r="F74">
         <v>12</v>
       </c>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
+      <c r="G74" s="8">
+        <v>42370</v>
+      </c>
+      <c r="H74" s="8">
+        <v>42339</v>
+      </c>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
@@ -13350,8 +14497,12 @@
       <c r="F75">
         <v>12</v>
       </c>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
+      <c r="G75" s="8">
+        <v>42401</v>
+      </c>
+      <c r="H75" s="8">
+        <v>42339</v>
+      </c>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
@@ -13375,6 +14526,12 @@
       <c r="F76">
         <v>12</v>
       </c>
+      <c r="G76" s="8">
+        <v>42430</v>
+      </c>
+      <c r="H76" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
@@ -13396,6 +14553,12 @@
       <c r="F77">
         <v>12</v>
       </c>
+      <c r="G77" s="8">
+        <v>42461</v>
+      </c>
+      <c r="H77" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
@@ -13417,6 +14580,12 @@
       <c r="F78">
         <v>12</v>
       </c>
+      <c r="G78" s="8">
+        <v>42491</v>
+      </c>
+      <c r="H78" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
@@ -13438,6 +14607,12 @@
       <c r="F79">
         <v>12</v>
       </c>
+      <c r="G79" s="8">
+        <v>42522</v>
+      </c>
+      <c r="H79" s="8">
+        <v>42339</v>
+      </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -13459,8 +14634,14 @@
       <c r="F80">
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" s="8">
+        <v>42552</v>
+      </c>
+      <c r="H80" s="8">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>4</v>
       </c>
@@ -13479,6 +14660,12 @@
       </c>
       <c r="F81">
         <v>12</v>
+      </c>
+      <c r="G81" s="8">
+        <v>42583</v>
+      </c>
+      <c r="H81" s="8">
+        <v>42339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>